<commit_message>
Updated the ps3.xlsx file with the new data
</commit_message>
<xml_diff>
--- a/ps3/ps3.xlsx
+++ b/ps3/ps3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johanoelgaard/My Drive/04 Økonomi/08 Financial Economics/03 Problem Sets/ECON136/ps3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE45D75-C911-C943-9351-59E94D12F050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905EE443-D161-754E-9025-3AEF227C3FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2115212E-5A06-0C47-8CE8-8E72B33899CD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2115212E-5A06-0C47-8CE8-8E72B33899CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -265,15 +265,15 @@
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="171" formatCode="[$$-409]#,##0.000"/>
-    <numFmt numFmtId="173" formatCode="[$$-409]#,##0"/>
-    <numFmt numFmtId="180" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="191" formatCode="[$$-409]#,##0.00000"/>
-    <numFmt numFmtId="193" formatCode="0.000%"/>
-    <numFmt numFmtId="194" formatCode="0.0000%"/>
-    <numFmt numFmtId="198" formatCode="0.000"/>
-    <numFmt numFmtId="199" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;???_ ;_-@_ "/>
-    <numFmt numFmtId="203" formatCode="_-[$$-409]* #,##0.0000000_ ;_-[$$-409]* \-#,##0.0000000\ ;_-[$$-409]* &quot;-&quot;???_ ;_-@_ "/>
+    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.000"/>
+    <numFmt numFmtId="171" formatCode="[$$-409]#,##0"/>
+    <numFmt numFmtId="172" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00000"/>
+    <numFmt numFmtId="174" formatCode="0.000%"/>
+    <numFmt numFmtId="175" formatCode="0.0000%"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;???_ ;_-@_ "/>
+    <numFmt numFmtId="178" formatCode="_-[$$-409]* #,##0.0000000_ ;_-[$$-409]* \-#,##0.0000000\ ;_-[$$-409]* &quot;-&quot;???_ ;_-@_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -370,30 +370,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F976EF19-2D6F-1944-9AAD-A2EFA326274F}">
   <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D210" sqref="D208:D210"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,24 +725,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -777,7 +777,7 @@
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -803,15 +803,15 @@
         <v>1</v>
       </c>
       <c r="B13" s="7">
-        <f>$B$9</f>
+        <f t="shared" ref="B13:B22" si="0">$B$9</f>
         <v>100</v>
       </c>
       <c r="C13" s="10">
-        <f>1/(1+$B$7)^A13</f>
+        <f t="shared" ref="C13:C22" si="1">1/(1+$B$7)^A13</f>
         <v>0.90909090909090906</v>
       </c>
       <c r="D13" s="9">
-        <f>B13*C13</f>
+        <f t="shared" ref="D13:D22" si="2">B13*C13</f>
         <v>90.909090909090907</v>
       </c>
       <c r="E13" s="8">
@@ -821,163 +821,163 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f>A13+1</f>
+        <f t="shared" ref="A14:A22" si="3">A13+1</f>
         <v>2</v>
       </c>
       <c r="B14" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C14" s="10">
-        <f>1/(1+$B$7)^A14</f>
+        <f t="shared" si="1"/>
         <v>0.82644628099173545</v>
       </c>
       <c r="D14" s="9">
-        <f>B14*C14</f>
+        <f t="shared" si="2"/>
         <v>82.644628099173545</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f>A14+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B15" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C15" s="10">
-        <f>1/(1+$B$7)^A15</f>
+        <f t="shared" si="1"/>
         <v>0.75131480090157754</v>
       </c>
       <c r="D15" s="9">
-        <f>B15*C15</f>
+        <f t="shared" si="2"/>
         <v>75.131480090157751</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>A15+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B16" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C16" s="10">
-        <f>1/(1+$B$7)^A16</f>
+        <f t="shared" si="1"/>
         <v>0.68301345536507052</v>
       </c>
       <c r="D16" s="9">
-        <f>B16*C16</f>
+        <f t="shared" si="2"/>
         <v>68.301345536507057</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>A16+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B17" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C17" s="10">
-        <f>1/(1+$B$7)^A17</f>
+        <f t="shared" si="1"/>
         <v>0.62092132305915493</v>
       </c>
       <c r="D17" s="9">
-        <f>B17*C17</f>
+        <f t="shared" si="2"/>
         <v>62.092132305915491</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>A17+1</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B18" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C18" s="10">
-        <f>1/(1+$B$7)^A18</f>
+        <f t="shared" si="1"/>
         <v>0.56447393005377722</v>
       </c>
       <c r="D18" s="9">
-        <f>B18*C18</f>
+        <f t="shared" si="2"/>
         <v>56.44739300537772</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f>A18+1</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B19" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C19" s="10">
-        <f>1/(1+$B$7)^A19</f>
+        <f t="shared" si="1"/>
         <v>0.51315811823070645</v>
       </c>
       <c r="D19" s="9">
-        <f>B19*C19</f>
+        <f t="shared" si="2"/>
         <v>51.315811823070646</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B20" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C20" s="10">
-        <f>1/(1+$B$7)^A20</f>
+        <f t="shared" si="1"/>
         <v>0.46650738020973315</v>
       </c>
       <c r="D20" s="9">
-        <f>B20*C20</f>
+        <f t="shared" si="2"/>
         <v>46.650738020973314</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B21" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C21" s="10">
-        <f>1/(1+$B$7)^A21</f>
+        <f t="shared" si="1"/>
         <v>0.42409761837248466</v>
       </c>
       <c r="D21" s="9">
-        <f>B21*C21</f>
+        <f t="shared" si="2"/>
         <v>42.409761837248467</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B22" s="7">
-        <f>$B$9</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C22" s="10">
-        <f>1/(1+$B$7)^A22</f>
+        <f t="shared" si="1"/>
         <v>0.38554328942953148</v>
       </c>
       <c r="D22" s="9">
-        <f>B22*C22</f>
+        <f t="shared" si="2"/>
         <v>38.554328942953148</v>
       </c>
       <c r="G22" s="11"/>
@@ -986,7 +986,7 @@
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -998,18 +998,18 @@
         <f>PV($B$7,$B$8,$B$9,$B$10,0)</f>
         <v>-614.45671057046854</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1034,16 +1034,16 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>0</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>0</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="14">
         <v>80000</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="14">
         <v>175000</v>
       </c>
     </row>
@@ -1051,16 +1051,16 @@
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="15">
         <v>0</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="15">
         <v>4</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>10</v>
       </c>
     </row>
@@ -1068,21 +1068,21 @@
       <c r="A33" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>1200000</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>1600000</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1109,25 +1109,25 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <f>-PV($B36,B$32,B$31,B$33,0)</f>
         <v>1200000</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="16">
         <f>-PV($B36,C$32,C$31,C$33,0)</f>
         <v>1316323.9596670112</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="16">
         <f>$D$31/B36</f>
         <v>1600000</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="16">
         <f>-PV($B36,E$32,E$31,E$33,0)</f>
         <v>1351303.6126073422</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1154,19 +1154,19 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="17">
+      <c r="B45" s="16">
         <f>-PV($B42,B$32,B$31,B$33,0)</f>
         <v>1200000</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="16">
         <f>-PV($B42,C$32,C$31,C$33,0)</f>
         <v>1133480.3377043144</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="16">
         <f>$D$31/B42</f>
         <v>888888.88888888888</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="16">
         <f>-PV($B42,E$32,E$31,E$33,0)</f>
         <v>1123090.0977028273</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       <c r="A51" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="14">
         <v>1000</v>
       </c>
     </row>
@@ -1241,18 +1241,18 @@
         <v>0.02</v>
       </c>
       <c r="C57" s="10">
-        <f>1/((1+($B57/$B$53))^$A57)</f>
+        <f t="shared" ref="C57:C66" si="4">1/((1+($B57/$B$53))^$A57)</f>
         <v>0.99009900990099009</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E57" s="19">
-        <f>$C57*$D57</f>
+      <c r="E57" s="18">
+        <f t="shared" ref="E57:E66" si="5">$C57*$D57</f>
         <v>24.752475247524753</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="19">
         <f>SUM(E57:E66)</f>
         <v>968.07314100701524</v>
       </c>
@@ -1266,15 +1266,15 @@
         <v>0.03</v>
       </c>
       <c r="C58" s="10">
-        <f>1/((1+($B58/$B$53))^$A58)</f>
+        <f t="shared" si="4"/>
         <v>0.9706617486471405</v>
       </c>
-      <c r="D58" s="15">
-        <f t="shared" ref="D58:D65" si="0">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E58" s="19">
-        <f>$C58*$D58</f>
+      <c r="D58" s="14">
+        <f t="shared" ref="D58:D65" si="6">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E58" s="18">
+        <f t="shared" si="5"/>
         <v>24.266543716178511</v>
       </c>
     </row>
@@ -1283,19 +1283,19 @@
         <f>A58+1</f>
         <v>3</v>
       </c>
-      <c r="B59" s="18">
+      <c r="B59" s="17">
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="C59" s="10">
-        <f>1/((1+($B59/$B$53))^$A59)</f>
+        <f t="shared" si="4"/>
         <v>0.94691020450444718</v>
       </c>
-      <c r="D59" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E59" s="19">
-        <f>$C59*$D59</f>
+      <c r="D59" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E59" s="18">
+        <f t="shared" si="5"/>
         <v>23.672755112611181</v>
       </c>
     </row>
@@ -1304,19 +1304,19 @@
         <f>A59+1</f>
         <v>4</v>
       </c>
-      <c r="B60" s="18">
+      <c r="B60" s="17">
         <v>4.1700000000000001E-2</v>
       </c>
       <c r="C60" s="10">
-        <f>1/((1+($B60/$B$53))^$A60)</f>
+        <f t="shared" si="4"/>
         <v>0.92077234618924586</v>
       </c>
-      <c r="D60" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E60" s="19">
-        <f>$C60*$D60</f>
+      <c r="D60" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E60" s="18">
+        <f t="shared" si="5"/>
         <v>23.019308654731148</v>
       </c>
     </row>
@@ -1325,129 +1325,129 @@
         <f>A60+1</f>
         <v>5</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="17">
         <v>4.5699999999999998E-2</v>
       </c>
       <c r="C61" s="10">
-        <f>1/((1+($B61/$B$53))^$A61)</f>
+        <f t="shared" si="4"/>
         <v>0.89318259684008927</v>
       </c>
-      <c r="D61" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E61" s="19">
-        <f>$C61*$D61</f>
+      <c r="D61" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E61" s="18">
+        <f t="shared" si="5"/>
         <v>22.32956492100223</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f t="shared" ref="A62:A66" si="1">A61+1</f>
+        <f t="shared" ref="A62:A66" si="7">A61+1</f>
         <v>6</v>
       </c>
-      <c r="B62" s="18">
+      <c r="B62" s="17">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="C62" s="10">
-        <f>1/((1+($B62/$B$53))^$A62)</f>
+        <f t="shared" si="4"/>
         <v>0.86482497619650811</v>
       </c>
-      <c r="D62" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E62" s="19">
-        <f>$C62*$D62</f>
+      <c r="D62" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E62" s="18">
+        <f t="shared" si="5"/>
         <v>21.620624404912704</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="B63" s="18">
+      <c r="B63" s="17">
         <v>5.1900000000000002E-2</v>
       </c>
       <c r="C63" s="10">
-        <f>1/((1+($B63/$B$53))^$A63)</f>
+        <f t="shared" si="4"/>
         <v>0.8358274486617927</v>
       </c>
-      <c r="D63" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E63" s="19">
-        <f>$C63*$D63</f>
+      <c r="D63" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E63" s="18">
+        <f t="shared" si="5"/>
         <v>20.895686216544817</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="B64" s="18">
+      <c r="B64" s="17">
         <v>5.4399999999999997E-2</v>
       </c>
       <c r="C64" s="10">
-        <f>1/((1+($B64/$B$53))^$A64)</f>
+        <f t="shared" si="4"/>
         <v>0.80678889953590782</v>
       </c>
-      <c r="D64" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E64" s="19">
-        <f>$C64*$D64</f>
+      <c r="D64" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E64" s="18">
+        <f t="shared" si="5"/>
         <v>20.169722488397696</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="B65" s="18">
+      <c r="B65" s="17">
         <v>5.6599999999999998E-2</v>
       </c>
       <c r="C65" s="10">
-        <f>1/((1+($B65/$B$53))^$A65)</f>
+        <f t="shared" si="4"/>
         <v>0.77789589152603877</v>
       </c>
-      <c r="D65" s="15">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E65" s="19">
-        <f>$C65*$D65</f>
+      <c r="D65" s="14">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="E65" s="18">
+        <f t="shared" si="5"/>
         <v>19.44739728815097</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="B66" s="18">
+      <c r="B66" s="17">
         <v>5.8599999999999999E-2</v>
       </c>
       <c r="C66" s="10">
-        <f>1/((1+($B66/$B$53))^$A66)</f>
+        <f t="shared" si="4"/>
         <v>0.74916981751898659</v>
       </c>
-      <c r="D66" s="15">
+      <c r="D66" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E66" s="19">
-        <f>$C66*$D66</f>
+      <c r="E66" s="18">
+        <f t="shared" si="5"/>
         <v>767.8990629569613</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       <c r="A70" t="s">
         <v>32</v>
       </c>
-      <c r="B70" s="18">
+      <c r="B70" s="17">
         <v>5.743669923384246E-2</v>
       </c>
     </row>
@@ -1488,23 +1488,23 @@
       <c r="A73">
         <v>1</v>
       </c>
-      <c r="B73" s="18">
-        <f>$B$70</f>
+      <c r="B73" s="17">
+        <f t="shared" ref="B73:B82" si="8">$B$70</f>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C73" s="10">
-        <f>1/((1+($B73/$B$53))^$A73)</f>
+        <f t="shared" ref="C73:C82" si="9">1/((1+($B73/$B$53))^$A73)</f>
         <v>0.97208336992567934</v>
       </c>
-      <c r="D73" s="15">
+      <c r="D73" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E73" s="19">
-        <f>$C73*$D73</f>
+      <c r="E73" s="18">
+        <f t="shared" ref="E73:E82" si="10">$C73*$D73</f>
         <v>24.302084248141984</v>
       </c>
-      <c r="F73" s="20">
+      <c r="F73" s="19">
         <f>SUM(E73:E82)-F57</f>
         <v>1.0732804355484404E-4</v>
       </c>
@@ -1514,20 +1514,20 @@
         <f>A73+1</f>
         <v>2</v>
       </c>
-      <c r="B74" s="18">
-        <f>$B$70</f>
+      <c r="B74" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C74" s="10">
-        <f>1/((1+($B74/$B$53))^$A74)</f>
+        <f t="shared" si="9"/>
         <v>0.94494607808606523</v>
       </c>
-      <c r="D74" s="15">
-        <f t="shared" ref="D74:D81" si="2">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E74" s="19">
-        <f>$C74*$D74</f>
+      <c r="D74" s="14">
+        <f t="shared" ref="D74:D81" si="11">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E74" s="18">
+        <f t="shared" si="10"/>
         <v>23.623651952151629</v>
       </c>
     </row>
@@ -1536,20 +1536,20 @@
         <f>A74+1</f>
         <v>3</v>
       </c>
-      <c r="B75" s="18">
-        <f>$B$70</f>
+      <c r="B75" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C75" s="10">
-        <f>1/((1+($B75/$B$53))^$A75)</f>
+        <f t="shared" si="9"/>
         <v>0.91856636798395641</v>
       </c>
-      <c r="D75" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E75" s="19">
-        <f>$C75*$D75</f>
+      <c r="D75" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E75" s="18">
+        <f t="shared" si="10"/>
         <v>22.96415919959891</v>
       </c>
     </row>
@@ -1558,20 +1558,20 @@
         <f>A75+1</f>
         <v>4</v>
       </c>
-      <c r="B76" s="18">
-        <f>$B$70</f>
+      <c r="B76" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C76" s="10">
-        <f>1/((1+($B76/$B$53))^$A76)</f>
+        <f t="shared" si="9"/>
         <v>0.89292309049023599</v>
       </c>
-      <c r="D76" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E76" s="19">
-        <f>$C76*$D76</f>
+      <c r="D76" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E76" s="18">
+        <f t="shared" si="10"/>
         <v>22.3230772622559</v>
       </c>
     </row>
@@ -1580,130 +1580,130 @@
         <f>A76+1</f>
         <v>5</v>
       </c>
-      <c r="B77" s="18">
-        <f>$B$70</f>
+      <c r="B77" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C77" s="10">
-        <f>1/((1+($B77/$B$53))^$A77)</f>
+        <f t="shared" si="9"/>
         <v>0.86799568688820095</v>
       </c>
-      <c r="D77" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E77" s="19">
-        <f>$C77*$D77</f>
+      <c r="D77" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E77" s="18">
+        <f t="shared" si="10"/>
         <v>21.699892172205022</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
-        <f t="shared" ref="A78:A82" si="3">A77+1</f>
+        <f t="shared" ref="A78:A82" si="12">A77+1</f>
         <v>6</v>
       </c>
-      <c r="B78" s="18">
-        <f>$B$70</f>
+      <c r="B78" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C78" s="10">
-        <f>1/((1+($B78/$B$53))^$A78)</f>
+        <f t="shared" si="9"/>
         <v>0.84376417239123724</v>
       </c>
-      <c r="D78" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E78" s="19">
-        <f>$C78*$D78</f>
+      <c r="D78" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E78" s="18">
+        <f t="shared" si="10"/>
         <v>21.094104309780931</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="B79" s="18">
-        <f>$B$70</f>
+      <c r="B79" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C79" s="10">
-        <f>1/((1+($B79/$B$53))^$A79)</f>
+        <f t="shared" si="9"/>
         <v>0.82020912012062575</v>
       </c>
-      <c r="D79" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E79" s="19">
-        <f>$C79*$D79</f>
+      <c r="D79" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E79" s="18">
+        <f t="shared" si="10"/>
         <v>20.505228003015645</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="B80" s="18">
-        <f>$B$70</f>
+      <c r="B80" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C80" s="10">
-        <f>1/((1+($B80/$B$53))^$A80)</f>
+        <f t="shared" si="9"/>
         <v>0.79731164553063416</v>
       </c>
-      <c r="D80" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E80" s="19">
-        <f>$C80*$D80</f>
+      <c r="D80" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E80" s="18">
+        <f t="shared" si="10"/>
         <v>19.932791138265856</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="B81" s="18">
-        <f>$B$70</f>
+      <c r="B81" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C81" s="10">
-        <f>1/((1+($B81/$B$53))^$A81)</f>
+        <f t="shared" si="9"/>
         <v>0.77505339126840755</v>
       </c>
-      <c r="D81" s="15">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="E81" s="19">
-        <f>$C81*$D81</f>
+      <c r="D81" s="14">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E81" s="18">
+        <f t="shared" si="10"/>
         <v>19.376334781710188</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
-      <c r="B82" s="18">
-        <f>$B$70</f>
+      <c r="B82" s="17">
+        <f t="shared" si="8"/>
         <v>5.743669923384246E-2</v>
       </c>
       <c r="C82" s="10">
-        <f>1/((1+($B82/$B$53))^$A82)</f>
+        <f t="shared" si="9"/>
         <v>0.75341651245651975</v>
       </c>
-      <c r="D82" s="15">
+      <c r="D82" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E82" s="19">
-        <f>$C82*$D82</f>
+      <c r="E82" s="18">
+        <f t="shared" si="10"/>
         <v>772.25192526793273</v>
       </c>
     </row>
@@ -1716,16 +1716,16 @@
       <c r="A85" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B85" s="22">
+      <c r="B85" s="21">
         <f>RATE(B54,B51*B52/B53,-F57,B51)*2</f>
         <v>5.7436724720469443E-2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B86" s="21"/>
+      <c r="B86" s="20"/>
     </row>
     <row r="96" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       <c r="A99" t="s">
         <v>39</v>
       </c>
-      <c r="B99" s="18">
+      <c r="B99" s="17">
         <f>$B$85</f>
         <v>5.7436724720469443E-2</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="A100" t="s">
         <v>24</v>
       </c>
-      <c r="B100" s="14">
+      <c r="B100" s="13">
         <f>F57</f>
         <v>968.07314100701524</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="D102" t="s">
         <v>48</v>
       </c>
-      <c r="E102" s="23" t="s">
+      <c r="E102" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1782,15 +1782,15 @@
         <f t="array" ref="B103:B112">$D$57:$D$66</f>
         <v>25</v>
       </c>
-      <c r="C103" s="24">
-        <f>$A103*(($B103/((1+($B$99/$B$98))^$A103))/$B$100)</f>
+      <c r="C103" s="23">
+        <f t="shared" ref="C103:C112" si="13">$A103*(($B103/((1+($B$99/$B$98))^$A103))/$B$100)</f>
         <v>2.5103561825730147E-2</v>
       </c>
-      <c r="D103" s="23">
+      <c r="D103" s="22">
         <f>1/$B$98</f>
         <v>0.5</v>
       </c>
-      <c r="E103" s="23">
+      <c r="E103" s="22">
         <f>D103*SUM(C103:C112)</f>
         <v>4.4752312900872226</v>
       </c>
@@ -1802,8 +1802,8 @@
       <c r="B104" s="7">
         <v>25</v>
       </c>
-      <c r="C104" s="24">
-        <f>$A104*(($B104/((1+($B$99/$B$98))^$A104))/$B$100)</f>
+      <c r="C104" s="23">
+        <f t="shared" si="13"/>
         <v>4.8805509348805468E-2</v>
       </c>
     </row>
@@ -1814,8 +1814,8 @@
       <c r="B105" s="7">
         <v>25</v>
       </c>
-      <c r="C105" s="24">
-        <f>$A105*(($B105/((1+($B$99/$B$98))^$A105))/$B$100)</f>
+      <c r="C105" s="23">
+        <f t="shared" si="13"/>
         <v>7.1164535116533936E-2</v>
       </c>
     </row>
@@ -1826,8 +1826,8 @@
       <c r="B106" s="7">
         <v>25</v>
       </c>
-      <c r="C106" s="24">
-        <f>$A106*(($B106/((1+($B$99/$B$98))^$A106))/$B$100)</f>
+      <c r="C106" s="23">
+        <f t="shared" si="13"/>
         <v>9.2237147011106052E-2</v>
       </c>
     </row>
@@ -1838,8 +1838,8 @@
       <c r="B107" s="7">
         <v>25</v>
       </c>
-      <c r="C107" s="24">
-        <f>$A107*(($B107/((1+($B$99/$B$98))^$A107))/$B$100)</f>
+      <c r="C107" s="23">
+        <f t="shared" si="13"/>
         <v>0.1120777444852377</v>
       </c>
     </row>
@@ -1850,8 +1850,8 @@
       <c r="B108" s="7">
         <v>25</v>
       </c>
-      <c r="C108" s="24">
-        <f>$A108*(($B108/((1+($B$99/$B$98))^$A108))/$B$100)</f>
+      <c r="C108" s="23">
+        <f t="shared" si="13"/>
         <v>0.13073869224392112</v>
       </c>
     </row>
@@ -1862,8 +1862,8 @@
       <c r="B109" s="7">
         <v>25</v>
       </c>
-      <c r="C109" s="24">
-        <f>$A109*(($B109/((1+($B$99/$B$98))^$A109))/$B$100)</f>
+      <c r="C109" s="23">
+        <f t="shared" si="13"/>
         <v>0.14827039145546284</v>
       </c>
     </row>
@@ -1874,8 +1874,8 @@
       <c r="B110" s="7">
         <v>25</v>
       </c>
-      <c r="C110" s="24">
-        <f>$A110*(($B110/((1+($B$99/$B$98))^$A110))/$B$100)</f>
+      <c r="C110" s="23">
+        <f t="shared" si="13"/>
         <v>0.1647213485723335</v>
       </c>
     </row>
@@ -1886,8 +1886,8 @@
       <c r="B111" s="7">
         <v>25</v>
       </c>
-      <c r="C111" s="24">
-        <f>$A111*(($B111/((1+($B$99/$B$98))^$A111))/$B$100)</f>
+      <c r="C111" s="23">
+        <f t="shared" si="13"/>
         <v>0.18013824183978466</v>
       </c>
     </row>
@@ -1898,13 +1898,13 @@
       <c r="B112" s="7">
         <v>1025</v>
       </c>
-      <c r="C112" s="24">
-        <f>$A112*(($B112/((1+($B$99/$B$98))^$A112))/$B$100)</f>
+      <c r="C112" s="23">
+        <f t="shared" si="13"/>
         <v>7.9772054082755304</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
+      <c r="A114" s="12" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       <c r="A116" t="s">
         <v>45</v>
       </c>
-      <c r="B116" s="23">
+      <c r="B116" s="22">
         <f>E103/(1+(B99/B98))</f>
         <v>4.3502978597752433</v>
       </c>
@@ -1921,13 +1921,13 @@
       <c r="A117" t="s">
         <v>44</v>
       </c>
-      <c r="B117" s="23">
+      <c r="B117" s="22">
         <f>MDURATION(DATE(2024,2,15),DATE(2029,2,15),5%,B99,2)</f>
         <v>4.3502978598045008</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
+      <c r="A119" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1944,7 +1944,7 @@
       <c r="D121" t="s">
         <v>48</v>
       </c>
-      <c r="E121" s="23" t="s">
+      <c r="E121" s="22" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1957,15 +1957,15 @@
         <f t="array" ref="B122:B131">$D$57:$D$66</f>
         <v>25</v>
       </c>
-      <c r="C122" s="24">
+      <c r="C122" s="23">
         <f>($A122^2 + $A122)*(($B122/((1+($B$99/$B$98))^$A122))/$B$100)</f>
         <v>5.0207123651460295E-2</v>
       </c>
-      <c r="D122" s="23">
+      <c r="D122" s="22">
         <f>1/(($B$98^2)*(1+($B$99/$B$98))^2)</f>
         <v>0.23623651366872681</v>
       </c>
-      <c r="E122" s="23">
+      <c r="E122" s="22">
         <f>D122*SUM(C122:C131)</f>
         <v>22.38326840494355</v>
       </c>
@@ -1977,8 +1977,8 @@
       <c r="B123" s="7">
         <v>25</v>
       </c>
-      <c r="C123" s="24">
-        <f t="shared" ref="C123:C131" si="4">($A123^2 + $A123)*(($B123/((1+($B$99/$B$98))^$A123))/$B$100)</f>
+      <c r="C123" s="23">
+        <f t="shared" ref="C123:C131" si="14">($A123^2 + $A123)*(($B123/((1+($B$99/$B$98))^$A123))/$B$100)</f>
         <v>0.14641652804641642</v>
       </c>
     </row>
@@ -1989,8 +1989,8 @@
       <c r="B124" s="7">
         <v>25</v>
       </c>
-      <c r="C124" s="24">
-        <f t="shared" si="4"/>
+      <c r="C124" s="23">
+        <f t="shared" si="14"/>
         <v>0.28465814046613575</v>
       </c>
     </row>
@@ -2001,8 +2001,8 @@
       <c r="B125" s="7">
         <v>25</v>
       </c>
-      <c r="C125" s="24">
-        <f t="shared" si="4"/>
+      <c r="C125" s="23">
+        <f t="shared" si="14"/>
         <v>0.46118573505553029</v>
       </c>
     </row>
@@ -2013,8 +2013,8 @@
       <c r="B126" s="7">
         <v>25</v>
       </c>
-      <c r="C126" s="24">
-        <f t="shared" si="4"/>
+      <c r="C126" s="23">
+        <f t="shared" si="14"/>
         <v>0.6724664669114262</v>
       </c>
     </row>
@@ -2025,8 +2025,8 @@
       <c r="B127" s="7">
         <v>25</v>
       </c>
-      <c r="C127" s="24">
-        <f t="shared" si="4"/>
+      <c r="C127" s="23">
+        <f t="shared" si="14"/>
         <v>0.91517084570744778</v>
       </c>
     </row>
@@ -2037,8 +2037,8 @@
       <c r="B128" s="7">
         <v>25</v>
       </c>
-      <c r="C128" s="24">
-        <f t="shared" si="4"/>
+      <c r="C128" s="23">
+        <f t="shared" si="14"/>
         <v>1.1861631316437027</v>
       </c>
     </row>
@@ -2049,8 +2049,8 @@
       <c r="B129" s="7">
         <v>25</v>
       </c>
-      <c r="C129" s="24">
-        <f t="shared" si="4"/>
+      <c r="C129" s="23">
+        <f t="shared" si="14"/>
         <v>1.4824921371510016</v>
       </c>
     </row>
@@ -2061,8 +2061,8 @@
       <c r="B130" s="7">
         <v>25</v>
       </c>
-      <c r="C130" s="24">
-        <f t="shared" si="4"/>
+      <c r="C130" s="23">
+        <f t="shared" si="14"/>
         <v>1.8013824183978466</v>
       </c>
     </row>
@@ -2073,13 +2073,13 @@
       <c r="B131" s="7">
         <v>1025</v>
       </c>
-      <c r="C131" s="24">
-        <f t="shared" si="4"/>
+      <c r="C131" s="23">
+        <f t="shared" si="14"/>
         <v>87.749259491030841</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A144" s="13" t="s">
+      <c r="A144" s="12" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2120,18 +2120,18 @@
         <v>0.03</v>
       </c>
       <c r="C148" s="10">
-        <f>1/((1+($B148/$B$53))^$A148)</f>
+        <f t="shared" ref="C148:C157" si="15">1/((1+($B148/$B$53))^$A148)</f>
         <v>0.98522167487684742</v>
       </c>
-      <c r="D148" s="15">
+      <c r="D148" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E148" s="19">
-        <f>$C148*$D148</f>
+      <c r="E148" s="18">
+        <f t="shared" ref="E148:E157" si="16">$C148*$D148</f>
         <v>24.630541871921185</v>
       </c>
-      <c r="F148" s="20">
+      <c r="F148" s="19">
         <f>SUM(E148:E157)</f>
         <v>927.13994922839356</v>
       </c>
@@ -2145,15 +2145,15 @@
         <v>0.04</v>
       </c>
       <c r="C149" s="10">
-        <f>1/((1+($B149/$B$53))^$A149)</f>
+        <f t="shared" si="15"/>
         <v>0.96116878123798544</v>
       </c>
-      <c r="D149" s="15">
-        <f t="shared" ref="D149:D156" si="5">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E149" s="19">
-        <f>$C149*$D149</f>
+      <c r="D149" s="14">
+        <f t="shared" ref="D149:D156" si="17">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E149" s="18">
+        <f t="shared" si="16"/>
         <v>24.029219530949636</v>
       </c>
     </row>
@@ -2162,19 +2162,19 @@
         <f>A149+1</f>
         <v>3</v>
       </c>
-      <c r="B150" s="18">
+      <c r="B150" s="17">
         <v>4.6700000000000005E-2</v>
       </c>
       <c r="C150" s="10">
-        <f>1/((1+($B150/$B$53))^$A150)</f>
+        <f t="shared" si="15"/>
         <v>0.9330983432004919</v>
       </c>
-      <c r="D150" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E150" s="19">
-        <f>$C150*$D150</f>
+      <c r="D150" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E150" s="18">
+        <f t="shared" si="16"/>
         <v>23.327458580012298</v>
       </c>
     </row>
@@ -2183,19 +2183,19 @@
         <f>A150+1</f>
         <v>4</v>
       </c>
-      <c r="B151" s="18">
+      <c r="B151" s="17">
         <v>5.1700000000000003E-2</v>
       </c>
       <c r="C151" s="10">
-        <f>1/((1+($B151/$B$53))^$A151)</f>
+        <f t="shared" si="15"/>
         <v>0.90295175999887423</v>
       </c>
-      <c r="D151" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E151" s="19">
-        <f>$C151*$D151</f>
+      <c r="D151" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E151" s="18">
+        <f t="shared" si="16"/>
         <v>22.573793999971855</v>
       </c>
     </row>
@@ -2204,129 +2204,129 @@
         <f>A151+1</f>
         <v>5</v>
       </c>
-      <c r="B152" s="18">
+      <c r="B152" s="17">
         <v>5.57E-2</v>
       </c>
       <c r="C152" s="10">
-        <f>1/((1+($B152/$B$53))^$A152)</f>
+        <f t="shared" si="15"/>
         <v>0.87166839361742754</v>
       </c>
-      <c r="D152" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E152" s="19">
-        <f>$C152*$D152</f>
+      <c r="D152" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E152" s="18">
+        <f t="shared" si="16"/>
         <v>21.79170984043569</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
-        <f t="shared" ref="A153:A157" si="6">A152+1</f>
+        <f t="shared" ref="A153:A157" si="18">A152+1</f>
         <v>6</v>
       </c>
-      <c r="B153" s="18">
+      <c r="B153" s="17">
         <v>5.9000000000000004E-2</v>
       </c>
       <c r="C153" s="10">
-        <f>1/((1+($B153/$B$53))^$A153)</f>
+        <f t="shared" si="15"/>
         <v>0.83992768098694681</v>
       </c>
-      <c r="D153" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E153" s="19">
-        <f>$C153*$D153</f>
+      <c r="D153" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E153" s="18">
+        <f t="shared" si="16"/>
         <v>20.998192024673671</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
-      <c r="B154" s="18">
+      <c r="B154" s="17">
         <v>6.1900000000000004E-2</v>
       </c>
       <c r="C154" s="10">
-        <f>1/((1+($B154/$B$53))^$A154)</f>
+        <f t="shared" si="15"/>
         <v>0.80786125382003782</v>
       </c>
-      <c r="D154" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E154" s="19">
-        <f>$C154*$D154</f>
+      <c r="D154" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E154" s="18">
+        <f t="shared" si="16"/>
         <v>20.196531345500944</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
-      <c r="B155" s="18">
+      <c r="B155" s="17">
         <v>6.4399999999999999E-2</v>
       </c>
       <c r="C155" s="10">
-        <f>1/((1+($B155/$B$53))^$A155)</f>
+        <f t="shared" si="15"/>
         <v>0.77604903306172346</v>
       </c>
-      <c r="D155" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E155" s="19">
-        <f>$C155*$D155</f>
+      <c r="D155" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E155" s="18">
+        <f t="shared" si="16"/>
         <v>19.401225826543087</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
-      <c r="B156" s="18">
+      <c r="B156" s="17">
         <v>6.6599999999999993E-2</v>
       </c>
       <c r="C156" s="10">
-        <f>1/((1+($B156/$B$53))^$A156)</f>
+        <f t="shared" si="15"/>
         <v>0.74466704635557901</v>
       </c>
-      <c r="D156" s="15">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="E156" s="19">
-        <f>$C156*$D156</f>
+      <c r="D156" s="14">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="E156" s="18">
+        <f t="shared" si="16"/>
         <v>18.616676158889476</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="B157" s="18">
+      <c r="B157" s="17">
         <v>6.8599999999999994E-2</v>
       </c>
       <c r="C157" s="10">
-        <f>1/((1+($B157/$B$53))^$A157)</f>
+        <f t="shared" si="15"/>
         <v>0.71373131712145932</v>
       </c>
-      <c r="D157" s="15">
+      <c r="D157" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E157" s="19">
-        <f>$C157*$D157</f>
+      <c r="E157" s="18">
+        <f t="shared" si="16"/>
         <v>731.57460004949576</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A159" s="13" t="s">
+      <c r="A159" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2367,18 +2367,18 @@
         <v>0.01</v>
       </c>
       <c r="C163" s="10">
-        <f>1/((1+($B163/$B$53))^$A163)</f>
+        <f t="shared" ref="C163:C172" si="19">1/((1+($B163/$B$53))^$A163)</f>
         <v>0.99502487562189068</v>
       </c>
-      <c r="D163" s="15">
+      <c r="D163" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E163" s="19">
-        <f>$C163*$D163</f>
+      <c r="E163" s="18">
+        <f t="shared" ref="E163:E172" si="20">$C163*$D163</f>
         <v>24.875621890547269</v>
       </c>
-      <c r="F163" s="20">
+      <c r="F163" s="19">
         <f>SUM(E163:E172)</f>
         <v>1011.1640405377015</v>
       </c>
@@ -2392,15 +2392,15 @@
         <v>1.9999999999999997E-2</v>
       </c>
       <c r="C164" s="10">
-        <f>1/((1+($B164/$B$53))^$A164)</f>
+        <f t="shared" si="19"/>
         <v>0.98029604940692083</v>
       </c>
-      <c r="D164" s="15">
-        <f t="shared" ref="D164:D171" si="7">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E164" s="19">
-        <f>$C164*$D164</f>
+      <c r="D164" s="14">
+        <f t="shared" ref="D164:D171" si="21">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E164" s="18">
+        <f t="shared" si="20"/>
         <v>24.50740123517302</v>
       </c>
     </row>
@@ -2409,19 +2409,19 @@
         <f>A164+1</f>
         <v>3</v>
       </c>
-      <c r="B165" s="18">
+      <c r="B165" s="17">
         <v>2.6700000000000002E-2</v>
       </c>
       <c r="C165" s="10">
-        <f>1/((1+($B165/$B$53))^$A165)</f>
+        <f t="shared" si="19"/>
         <v>0.96099600999614299</v>
       </c>
-      <c r="D165" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E165" s="19">
-        <f>$C165*$D165</f>
+      <c r="D165" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E165" s="18">
+        <f t="shared" si="20"/>
         <v>24.024900249903574</v>
       </c>
     </row>
@@ -2430,19 +2430,19 @@
         <f>A165+1</f>
         <v>4</v>
       </c>
-      <c r="B166" s="18">
+      <c r="B166" s="17">
         <v>3.1699999999999999E-2</v>
       </c>
       <c r="C166" s="10">
-        <f>1/((1+($B166/$B$53))^$A166)</f>
+        <f t="shared" si="19"/>
         <v>0.9390347416970215</v>
       </c>
-      <c r="D166" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E166" s="19">
-        <f>$C166*$D166</f>
+      <c r="D166" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E166" s="18">
+        <f t="shared" si="20"/>
         <v>23.475868542425538</v>
       </c>
     </row>
@@ -2451,129 +2451,129 @@
         <f>A166+1</f>
         <v>5</v>
       </c>
-      <c r="B167" s="18">
+      <c r="B167" s="17">
         <v>3.5699999999999996E-2</v>
       </c>
       <c r="C167" s="10">
-        <f>1/((1+($B167/$B$53))^$A167)</f>
+        <f t="shared" si="19"/>
         <v>0.9153371627918816</v>
       </c>
-      <c r="D167" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E167" s="19">
-        <f>$C167*$D167</f>
+      <c r="D167" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E167" s="18">
+        <f t="shared" si="20"/>
         <v>22.883429069797039</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
-        <f t="shared" ref="A168:A172" si="8">A167+1</f>
+        <f t="shared" ref="A168:A172" si="22">A167+1</f>
         <v>6</v>
       </c>
-      <c r="B168" s="18">
+      <c r="B168" s="17">
         <v>3.9E-2</v>
       </c>
       <c r="C168" s="10">
-        <f>1/((1+($B168/$B$53))^$A168)</f>
+        <f t="shared" si="19"/>
         <v>0.89058754941023544</v>
       </c>
-      <c r="D168" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E168" s="19">
-        <f>$C168*$D168</f>
+      <c r="D168" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E168" s="18">
+        <f t="shared" si="20"/>
         <v>22.264688735255884</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
-      <c r="B169" s="18">
+      <c r="B169" s="17">
         <v>4.19E-2</v>
       </c>
       <c r="C169" s="10">
-        <f>1/((1+($B169/$B$53))^$A169)</f>
+        <f t="shared" si="19"/>
         <v>0.86490555350727827</v>
       </c>
-      <c r="D169" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E169" s="19">
-        <f>$C169*$D169</f>
+      <c r="D169" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E169" s="18">
+        <f t="shared" si="20"/>
         <v>21.622638837681958</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
-      <c r="B170" s="18">
+      <c r="B170" s="17">
         <v>4.4399999999999995E-2</v>
       </c>
       <c r="C170" s="10">
-        <f>1/((1+($B170/$B$53))^$A170)</f>
+        <f t="shared" si="19"/>
         <v>0.83890539440738188</v>
       </c>
-      <c r="D170" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E170" s="19">
-        <f>$C170*$D170</f>
+      <c r="D170" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E170" s="18">
+        <f t="shared" si="20"/>
         <v>20.972634860184549</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="B171" s="18">
+      <c r="B171" s="17">
         <v>4.6599999999999996E-2</v>
       </c>
       <c r="C171" s="10">
-        <f>1/((1+($B171/$B$53))^$A171)</f>
+        <f t="shared" si="19"/>
         <v>0.81278042001613571</v>
       </c>
-      <c r="D171" s="15">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="E171" s="19">
-        <f>$C171*$D171</f>
+      <c r="D171" s="14">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="E171" s="18">
+        <f t="shared" si="20"/>
         <v>20.319510500403393</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
-      <c r="B172" s="18">
+      <c r="B172" s="17">
         <v>4.8599999999999997E-2</v>
       </c>
       <c r="C172" s="10">
-        <f>1/((1+($B172/$B$53))^$A172)</f>
+        <f t="shared" si="19"/>
         <v>0.78655350889397968</v>
       </c>
-      <c r="D172" s="15">
+      <c r="D172" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E172" s="19">
-        <f>$C172*$D172</f>
+      <c r="E172" s="18">
+        <f t="shared" si="20"/>
         <v>806.21734661632922</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A174" s="13" t="s">
+      <c r="A174" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2581,19 +2581,19 @@
       <c r="A175" t="s">
         <v>53</v>
       </c>
-      <c r="B175" s="27">
+      <c r="B175" s="26">
         <f>(F163-F148)/(2*(B145)*$F$57)</f>
         <v>4.3397594536040849</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B176" s="25"/>
+      <c r="B176" s="24"/>
     </row>
     <row r="177" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A177" s="13" t="s">
+      <c r="A177" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B177" s="25"/>
+      <c r="B177" s="24"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C178" t="s">
@@ -2608,7 +2608,7 @@
         <f>-$B$116*B145*$F$57+$F$57</f>
         <v>925.95907587272814</v>
       </c>
-      <c r="C179" s="26">
+      <c r="C179" s="25">
         <f>B179-F148</f>
         <v>-1.1808733556654261</v>
       </c>
@@ -2621,16 +2621,16 @@
         <f>-$B$116*B160*$F$57+$F$57</f>
         <v>1010.1872061413023</v>
       </c>
-      <c r="C180" s="26">
+      <c r="C180" s="25">
         <f>B180-F163</f>
         <v>-0.97683439639911285</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A181" s="13"/>
+      <c r="A181" s="12"/>
     </row>
     <row r="182" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A182" s="13" t="s">
+      <c r="A182" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
         <f>(-$B$116*B145+0.5*$E$122*(B145^2))*$F$57+$F$57</f>
         <v>927.04250792026687</v>
       </c>
-      <c r="C184" s="26">
+      <c r="C184" s="25">
         <f>B184-F148</f>
         <v>-9.7441308126690274E-2</v>
       </c>
@@ -2660,13 +2660,13 @@
         <f>(-$B$116*B160+0.5*$E$122*(B160^2))*$F$57+$F$57</f>
         <v>1011.2706381888412</v>
       </c>
-      <c r="C185" s="26">
+      <c r="C185" s="25">
         <f>B185-F163</f>
         <v>0.10659765113973663</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A192" s="13" t="s">
+      <c r="A192" s="12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2674,7 +2674,7 @@
       <c r="A193" t="s">
         <v>50</v>
       </c>
-      <c r="B193" s="18">
+      <c r="B193" s="17">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
@@ -2707,18 +2707,18 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="C196" s="10">
-        <f>1/((1+($B196/$B$53))^$A196)</f>
+        <f t="shared" ref="C196:C205" si="23">1/((1+($B196/$B$53))^$A196)</f>
         <v>0.9888751545117429</v>
       </c>
-      <c r="D196" s="15">
+      <c r="D196" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E196" s="19">
-        <f>$C196*$D196</f>
+      <c r="E196" s="18">
+        <f t="shared" ref="E196:E205" si="24">$C196*$D196</f>
         <v>24.721878862793574</v>
       </c>
-      <c r="F196" s="20">
+      <c r="F196" s="19">
         <f>SUM(E196:E205)</f>
         <v>957.64235541085213</v>
       </c>
@@ -2732,15 +2732,15 @@
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="C197" s="10">
-        <f>1/((1+($B197/$B$53))^$A197)</f>
+        <f t="shared" si="23"/>
         <v>0.96827536541048043</v>
       </c>
-      <c r="D197" s="15">
-        <f t="shared" ref="D197:D204" si="9">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E197" s="19">
-        <f>$C197*$D197</f>
+      <c r="D197" s="14">
+        <f t="shared" ref="D197:D204" si="25">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E197" s="18">
+        <f t="shared" si="24"/>
         <v>24.206884135262012</v>
       </c>
     </row>
@@ -2749,19 +2749,19 @@
         <f>A197+1</f>
         <v>3</v>
       </c>
-      <c r="B198" s="18">
+      <c r="B198" s="17">
         <v>3.9200000000000006E-2</v>
       </c>
       <c r="C198" s="10">
-        <f>1/((1+($B198/$B$53))^$A198)</f>
+        <f t="shared" si="23"/>
         <v>0.94343181912848972</v>
       </c>
-      <c r="D198" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E198" s="19">
-        <f>$C198*$D198</f>
+      <c r="D198" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E198" s="18">
+        <f t="shared" si="24"/>
         <v>23.585795478212244</v>
       </c>
     </row>
@@ -2770,19 +2770,19 @@
         <f>A198+1</f>
         <v>4</v>
       </c>
-      <c r="B199" s="18">
+      <c r="B199" s="17">
         <v>4.4200000000000003E-2</v>
       </c>
       <c r="C199" s="10">
-        <f>1/((1+($B199/$B$53))^$A199)</f>
+        <f t="shared" si="23"/>
         <v>0.91627628609579004</v>
       </c>
-      <c r="D199" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E199" s="19">
-        <f>$C199*$D199</f>
+      <c r="D199" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E199" s="18">
+        <f t="shared" si="24"/>
         <v>22.906907152394751</v>
       </c>
     </row>
@@ -2791,129 +2791,129 @@
         <f>A199+1</f>
         <v>5</v>
       </c>
-      <c r="B200" s="18">
+      <c r="B200" s="17">
         <v>4.82E-2</v>
       </c>
       <c r="C200" s="10">
-        <f>1/((1+($B200/$B$53))^$A200)</f>
+        <f t="shared" si="23"/>
         <v>0.88774486585712731</v>
       </c>
-      <c r="D200" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E200" s="19">
-        <f>$C200*$D200</f>
+      <c r="D200" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E200" s="18">
+        <f t="shared" si="24"/>
         <v>22.193621646428184</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
-        <f t="shared" ref="A201:A205" si="10">A200+1</f>
+        <f t="shared" ref="A201:A205" si="26">A200+1</f>
         <v>6</v>
       </c>
-      <c r="B201" s="18">
+      <c r="B201" s="17">
         <v>5.1500000000000004E-2</v>
       </c>
       <c r="C201" s="10">
-        <f>1/((1+($B201/$B$53))^$A201)</f>
+        <f t="shared" si="23"/>
         <v>0.85852084858538835</v>
       </c>
-      <c r="D201" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E201" s="19">
-        <f>$C201*$D201</f>
+      <c r="D201" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E201" s="18">
+        <f t="shared" si="24"/>
         <v>21.463021214634708</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
-        <f t="shared" si="10"/>
+        <f t="shared" si="26"/>
         <v>7</v>
       </c>
-      <c r="B202" s="18">
+      <c r="B202" s="17">
         <v>5.4400000000000004E-2</v>
       </c>
       <c r="C202" s="10">
-        <f>1/((1+($B202/$B$53))^$A202)</f>
+        <f t="shared" si="23"/>
         <v>0.82873355760328304</v>
       </c>
-      <c r="D202" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E202" s="19">
-        <f>$C202*$D202</f>
+      <c r="D202" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E202" s="18">
+        <f t="shared" si="24"/>
         <v>20.718338940082077</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
-        <f t="shared" si="10"/>
+        <f t="shared" si="26"/>
         <v>8</v>
       </c>
-      <c r="B203" s="18">
+      <c r="B203" s="17">
         <v>5.6899999999999999E-2</v>
       </c>
       <c r="C203" s="10">
-        <f>1/((1+($B203/$B$53))^$A203)</f>
+        <f t="shared" si="23"/>
         <v>0.79897748264328194</v>
       </c>
-      <c r="D203" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E203" s="19">
-        <f>$C203*$D203</f>
+      <c r="D203" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E203" s="18">
+        <f t="shared" si="24"/>
         <v>19.97443706608205</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
-        <f t="shared" si="10"/>
+        <f t="shared" si="26"/>
         <v>9</v>
       </c>
-      <c r="B204" s="18">
+      <c r="B204" s="17">
         <v>5.91E-2</v>
       </c>
       <c r="C204" s="10">
-        <f>1/((1+($B204/$B$53))^$A204)</f>
+        <f t="shared" si="23"/>
         <v>0.76943690632236439</v>
       </c>
-      <c r="D204" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="E204" s="19">
-        <f>$C204*$D204</f>
+      <c r="D204" s="14">
+        <f t="shared" si="25"/>
+        <v>25</v>
+      </c>
+      <c r="E204" s="18">
+        <f t="shared" si="24"/>
         <v>19.23592265805911</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
-        <f t="shared" si="10"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
-      <c r="B205" s="18">
+      <c r="B205" s="17">
         <v>6.1100000000000002E-2</v>
       </c>
       <c r="C205" s="10">
-        <f>1/((1+($B205/$B$53))^$A205)</f>
+        <f t="shared" si="23"/>
         <v>0.74013224220185703</v>
       </c>
-      <c r="D205" s="15">
+      <c r="D205" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E205" s="19">
-        <f>$C205*$D205</f>
+      <c r="E205" s="18">
+        <f t="shared" si="24"/>
         <v>758.63554825690346</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A207" s="13" t="s">
+      <c r="A207" s="12" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2921,7 +2921,7 @@
       <c r="A208" t="s">
         <v>50</v>
       </c>
-      <c r="B208" s="18">
+      <c r="B208" s="17">
         <v>-2.5000000000000001E-3</v>
       </c>
     </row>
@@ -2954,18 +2954,18 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="C211" s="10">
-        <f>1/((1+($B211/$B$53))^$A211)</f>
+        <f t="shared" ref="C211:C220" si="27">1/((1+($B211/$B$53))^$A211)</f>
         <v>0.99132589838909535</v>
       </c>
-      <c r="D211" s="15">
+      <c r="D211" s="14">
         <f>$B$51*$B$52/$B$53</f>
         <v>25</v>
       </c>
-      <c r="E211" s="19">
-        <f>$C211*$D211</f>
+      <c r="E211" s="18">
+        <f t="shared" ref="E211:E220" si="28">$C211*$D211</f>
         <v>24.783147459727385</v>
       </c>
-      <c r="F211" s="20">
+      <c r="F211" s="19">
         <f>SUM(E211:E220)</f>
         <v>978.63874577184606</v>
       </c>
@@ -2979,15 +2979,15 @@
         <v>2.75E-2</v>
       </c>
       <c r="C212" s="10">
-        <f>1/((1+($B212/$B$53))^$A212)</f>
+        <f t="shared" si="27"/>
         <v>0.97305696488328641</v>
       </c>
-      <c r="D212" s="15">
-        <f t="shared" ref="D212:D219" si="11">$B$51*$B$52/$B$53</f>
-        <v>25</v>
-      </c>
-      <c r="E212" s="19">
-        <f>$C212*$D212</f>
+      <c r="D212" s="14">
+        <f t="shared" ref="D212:D219" si="29">$B$51*$B$52/$B$53</f>
+        <v>25</v>
+      </c>
+      <c r="E212" s="18">
+        <f t="shared" si="28"/>
         <v>24.326424122082159</v>
       </c>
     </row>
@@ -2996,19 +2996,19 @@
         <f>A212+1</f>
         <v>3</v>
       </c>
-      <c r="B213" s="18">
+      <c r="B213" s="17">
         <v>3.4200000000000001E-2</v>
       </c>
       <c r="C213" s="10">
-        <f>1/((1+($B213/$B$53))^$A213)</f>
+        <f t="shared" si="27"/>
         <v>0.95040571042476629</v>
       </c>
-      <c r="D213" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E213" s="19">
-        <f>$C213*$D213</f>
+      <c r="D213" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E213" s="18">
+        <f t="shared" si="28"/>
         <v>23.760142760619157</v>
       </c>
     </row>
@@ -3017,19 +3017,19 @@
         <f>A213+1</f>
         <v>4</v>
       </c>
-      <c r="B214" s="18">
+      <c r="B214" s="17">
         <v>3.9199999999999999E-2</v>
       </c>
       <c r="C214" s="10">
-        <f>1/((1+($B214/$B$53))^$A214)</f>
+        <f t="shared" si="27"/>
         <v>0.92529601719153554</v>
       </c>
-      <c r="D214" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E214" s="19">
-        <f>$C214*$D214</f>
+      <c r="D214" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E214" s="18">
+        <f t="shared" si="28"/>
         <v>23.132400429788387</v>
       </c>
     </row>
@@ -3038,129 +3038,129 @@
         <f>A214+1</f>
         <v>5</v>
       </c>
-      <c r="B215" s="18">
+      <c r="B215" s="17">
         <v>4.3199999999999995E-2</v>
       </c>
       <c r="C215" s="10">
-        <f>1/((1+($B215/$B$53))^$A215)</f>
+        <f t="shared" si="27"/>
         <v>0.89866034630968739</v>
       </c>
-      <c r="D215" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E215" s="19">
-        <f>$C215*$D215</f>
+      <c r="D215" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E215" s="18">
+        <f t="shared" si="28"/>
         <v>22.466508657742185</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216">
-        <f t="shared" ref="A216:A220" si="12">A215+1</f>
+        <f t="shared" ref="A216:A220" si="30">A215+1</f>
         <v>6</v>
       </c>
-      <c r="B216" s="18">
+      <c r="B216" s="17">
         <v>4.65E-2</v>
       </c>
       <c r="C216" s="10">
-        <f>1/((1+($B216/$B$53))^$A216)</f>
+        <f t="shared" si="27"/>
         <v>0.87118317643765275</v>
       </c>
-      <c r="D216" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E216" s="19">
-        <f>$C216*$D216</f>
+      <c r="D216" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E216" s="18">
+        <f t="shared" si="28"/>
         <v>21.77957941094132</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217">
-        <f t="shared" si="12"/>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
-      <c r="B217" s="18">
+      <c r="B217" s="17">
         <v>4.9399999999999999E-2</v>
       </c>
       <c r="C217" s="10">
-        <f>1/((1+($B217/$B$53))^$A217)</f>
+        <f t="shared" si="27"/>
         <v>0.84299082249065382</v>
       </c>
-      <c r="D217" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E217" s="19">
-        <f>$C217*$D217</f>
+      <c r="D217" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E217" s="18">
+        <f t="shared" si="28"/>
         <v>21.074770562266345</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218">
-        <f t="shared" si="12"/>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
-      <c r="B218" s="18">
+      <c r="B218" s="17">
         <v>5.1899999999999995E-2</v>
       </c>
       <c r="C218" s="10">
-        <f>1/((1+($B218/$B$53))^$A218)</f>
+        <f t="shared" si="27"/>
         <v>0.81468633818586955</v>
       </c>
-      <c r="D218" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E218" s="19">
-        <f>$C218*$D218</f>
+      <c r="D218" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E218" s="18">
+        <f t="shared" si="28"/>
         <v>20.367158454646738</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219">
-        <f t="shared" si="12"/>
+        <f t="shared" si="30"/>
         <v>9</v>
       </c>
-      <c r="B219" s="18">
+      <c r="B219" s="17">
         <v>5.4099999999999995E-2</v>
       </c>
       <c r="C219" s="10">
-        <f>1/((1+($B219/$B$53))^$A219)</f>
+        <f t="shared" si="27"/>
         <v>0.78645833170965584</v>
       </c>
-      <c r="D219" s="15">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="E219" s="19">
-        <f>$C219*$D219</f>
+      <c r="D219" s="14">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="E219" s="18">
+        <f t="shared" si="28"/>
         <v>19.661458292741397</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220">
-        <f t="shared" si="12"/>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
-      <c r="B220" s="18">
+      <c r="B220" s="17">
         <v>5.6099999999999997E-2</v>
       </c>
       <c r="C220" s="10">
-        <f>1/((1+($B220/$B$53))^$A220)</f>
+        <f t="shared" si="27"/>
         <v>0.75832893231345455</v>
       </c>
-      <c r="D220" s="15">
+      <c r="D220" s="14">
         <f>$B$51*$B$52/$B$53+$B$51</f>
         <v>1025</v>
       </c>
-      <c r="E220" s="19">
-        <f>$C220*$D220</f>
+      <c r="E220" s="18">
+        <f t="shared" si="28"/>
         <v>777.28715562129094</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A222" s="13" t="s">
+      <c r="A222" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3168,27 +3168,27 @@
       <c r="A223" t="s">
         <v>53</v>
       </c>
-      <c r="B223" s="27">
+      <c r="B223" s="26">
         <f>(F211-F196)/(2*(B193)*$F$57)</f>
         <v>4.3377694249740113</v>
       </c>
-      <c r="D223" s="14">
+      <c r="D223" s="13">
         <f>(F211-F196)</f>
         <v>20.996390360993928</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B224" s="25"/>
-      <c r="D224" s="14">
+      <c r="B224" s="24"/>
+      <c r="D224" s="13">
         <f>(2*(B193)*$F$57)</f>
         <v>4.8403657050350759</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A225" s="13" t="s">
+      <c r="A225" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B225" s="25"/>
+      <c r="B225" s="24"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C226" t="s">
@@ -3203,11 +3203,11 @@
         <f>-$B$116*B193*$F$57+$F$57</f>
         <v>957.54462472344346</v>
       </c>
-      <c r="C227" s="26">
+      <c r="C227" s="25">
         <f>B227-F196</f>
         <v>-9.7730687408670747E-2</v>
       </c>
-      <c r="D227" s="29"/>
+      <c r="D227" s="27"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
@@ -3217,16 +3217,16 @@
         <f>-$B$116*B208*$F$57+$F$57</f>
         <v>978.60165729058701</v>
       </c>
-      <c r="C228" s="26">
+      <c r="C228" s="25">
         <f>B228-F211</f>
         <v>-3.7088481259047512E-2</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A229" s="13"/>
+      <c r="A229" s="12"/>
     </row>
     <row r="230" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A230" s="13" t="s">
+      <c r="A230" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3243,11 +3243,11 @@
         <f>(-$B$116*B193+0.5*$E$122*(B193^2))*$F$57+$F$57</f>
         <v>957.61233922641463</v>
       </c>
-      <c r="C232" s="26">
+      <c r="C232" s="25">
         <f>B232-F196</f>
         <v>-3.001618443749976E-2</v>
       </c>
-      <c r="D232" s="29"/>
+      <c r="D232" s="27"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
@@ -3257,7 +3257,7 @@
         <f>(-$B$116*B208+0.5*$E$122*(B208^2))*$F$57+$F$57</f>
         <v>978.66937179355818</v>
       </c>
-      <c r="C233" s="26">
+      <c r="C233" s="25">
         <f>B233-F211</f>
         <v>3.0626021712123475E-2</v>
       </c>

</xml_diff>